<commit_message>
Criando serviço de importação
</commit_message>
<xml_diff>
--- a/src/main/resources/carga-inicial-doadores.xlsx
+++ b/src/main/resources/carga-inicial-doadores.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Campos Maia" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Quadra Coberta" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="397">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -340,7 +341,7 @@
     <t xml:space="preserve">99220-4661</t>
   </si>
   <si>
-    <t xml:space="preserve">ChIJ-1Xg_WrwzJQRyo_DfJo-Two</t>
+    <t xml:space="preserve">ChIJ-1Xg_WrwzJQRyo_DfJo-TWo</t>
   </si>
   <si>
     <t xml:space="preserve">Diego Benedito dos Santos</t>
@@ -500,16 +501,776 @@
   </si>
   <si>
     <t xml:space="preserve">ChIJUdMwJhXwzJQR2W-hyefzspU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Célia dos Santos Silva Almeida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3522-0358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Francisca Bicudo de Mello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quadra Coberta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJgRLUKT7wzJQRvdG_998BHP8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcia/José Renato Santos Clemente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99218-8537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDM3NiAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJqVVTnhXwzJQRrn7X_98Wf_4Q-AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efigênia Leme da Silva Marcondes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99116-8005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJh5SBBBXwzJQRtnaLnq3ThVU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lourdes Narezi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-3230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Álvaro Leme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJr4gfYRXwzJQReOvoKpPhb_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wilson Caetano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-1650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJVws2XhXwzJQRT0qHlqFIl2g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana Aboud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99177-5585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ1UvRMRXwzJQRDnecqmIZBN8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alarico Filho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99207-8084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Professor Demétrio Boueri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ4_GM0j_wzJQR_Shxye3R4LY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauro Fernando Soares Ribeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-4121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJYV9gFhXwzJQReXVKJzcYJwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenita de Azevedo Freitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-2184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJdzLjGRXwzJQRBftquE2IrmA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Francisco Roberto Martins Junior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99103-1805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Ignácio Henrique Romeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJg0wYJD7wzJQRkmT1W1OX_7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shirley Cezar Nogueira Brasil Maia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98822-8803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Manuel Cembranelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ7zfpEEDwzJQR_du0Szi8mh0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Carlos Marcelino Junior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97411-7662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Com, Augusto Marcondes Salgado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmdSLiBDb21lbmRhZG9yIEF1Z3VzdG8gTWFyY29uZGVzIFNhbGdhZG8sIDE3OCAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTE2MCwgQnJhemlsIhsSGQoUChIJJT_U-j_wzJQRYlguFVZPt2wQsgE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sidney Batista do Nascimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99174-1901</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Com. Augusto Marcondes Salgado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJgazxSxXwzJQRB9i3mRBSqEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria das Graças de Lima Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3527-5065</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Avenida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Abel Correia Guimarães</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ2VnGOhXwzJQRKMx3wu17psY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luiz Carlos Correard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-7953</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Avenida</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Abel Correia Guimarães</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJyWppt2rwzJQRYqduxvtzHE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terezinha de Jesus Campos da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-2268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Joaquim Rosa e Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ83H9GEDwzJQRdckBTa0rAFs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José de Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3527-8509</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Manoel Cembranelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ4yUWDBXwzJQRveR6S8KgGuw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neide Saraiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99150-0186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FUNDOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJmUULQhXwzJQRNIui-03ZCSQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonio Sebastiana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-6510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ63rlVRXwzJQRwsJNk67z3HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerollen Gonçalves Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99630-0794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJQ3pq_j_wzJQRVX0vdnejJdc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Luiza Novais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98163-3575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJS-4uOD7wzJQRqCDYmHG44Jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eunice de Oliveira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-4316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDM2NiAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJqVVTnhXwzJQRrn7X_98Wf_4Q7gI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Aparecida Gomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-9665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDQzNCAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJN-0eBBXwzJQR-hkfsGsoo0kQsgM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandra Mara dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3648-2215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDQ2MCAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJN-0eBBXwzJQR-hkfsGsoo0kQzAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angela Maria Queiroz de Morais </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3522-1198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDU2NSAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJN-0eBBXwzJQR-xkfsGsoo0kQtQQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberta Juliana da Fonseca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3522-1325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIGAR ANTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EllSLiBQcm9mLiBEZW3DqXRyaW8gQm91ZXJpLCA0NjAgLSBDaMOhY2FyYSBHYWxlZ2EsIFBpbmRhbW9uaGFuZ2FiYSAtIFNQLCAxMjQyMi0xNDAsIEJyYXppbCIbEhkKFAoSCbfQlxYV8MyUEZhZOKnb61M9EMwD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedito dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ek9SLiDDgWx2YXJvIExlbWUsIDE5NSAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTE1MCwgQnJhemlsIhsSGQoUChIJyW8RYBXwzJQRywK0uWkzKggQwwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Angela Mesquita Punzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99228-2704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ7ei_NxXwzJQRzxx3GLxHpz4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carmem Lúcia Corrêa Leite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99185-3797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Professor Fued Boueri</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (FORA DE ORDEM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJXRd1CEDwzJQRG7pU_ork0jQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafael Ribeiro Cavalcante de Souza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99101-7429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Fued Boueri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJUe0npGrwzJQR0T5Yb0MV3XE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telma Ogata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-1815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praça Marechal Castelo Branco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJMSve6G3wzJQRaWSKTyBLBf4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinaura Flora Azevedo dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3648-1330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenida Abel Corrêa Guimarães</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJTeSZIxXwzJQRjIYUHlpeCJU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regina Aparecida Rosas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3648-4482</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Avenida</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Abel Corrêa Guimarães</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ6URANhXwzJQRQeiO-kzdmb0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dijia Bueno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99665-1150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ73ovumrwzJQR6Z95MZ2-6fo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roma Braga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3648-6321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Dos Bentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MESMO LADO / Leite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJf-a14BXwzJQR7tyUk7iUMu8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice Apolinário Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-2618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJP_s93hXwzJQRLJluw9BXpjY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elisabeth Moura da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3643-1051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Praça Castelo Branco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJyauGdxXwzJQRwTIZ9rOunlI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-6630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJV_JL5z_wzJQRml2WGWzseLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Aparecida Santinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3527-8941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ek9SLiDDgWx2YXJvIExlbWUsIDQ4OCAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTE1MCwgQnJhemlsIhsSGQoUChIJ0QBJLhXwzJQReNDnejFe4O8Q6AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosimeire Campos de Araújo Frota </t>
+  </si>
+  <si>
+    <t xml:space="preserve">99105-9932</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJB9f_Sz7wzJQRgmrKmIfR0Ko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luíza Takara Martinaczo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-4462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJA8iWcBXwzJQRN0PjY_S0mEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliana de Jesus Marcondes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-1470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJl4sjhBXwzJQRNR1kehg5sfw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margarete Correa do Nascimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3645-4164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDM5MiAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJqVVTnhXwzJQRrn7X_98Wf_4QiAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renata de Souza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3645-6611</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Francisca Bicudo de Melo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EltSLiBGcmFuY2lzY2EgQmljdWRvIGRlIE1lbG8sIDQwNyAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTEzMCwgQnJhemlsIhsSGQoUChIJqVVTnhXwzJQRr37X_98Wf_4QlwM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edithe Ferreira Ramos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98187-0058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJhVFwtT_wzJQRle3gfNuLZnY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waldirene Machado Pereira dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-8441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ92t9tj_wzJQRhX_BVG9-_MI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscarina Souza dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-3803</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJmcSTsz_wzJQRvFgdHu6FIrQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juliana Salmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99670-1934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJLWvgF0DwzJQRfY0VCVdY0Vo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Major Joaquim Antonio de Melo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJk4x-3T_wzJQR8WsHi3VXLy0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luciana do Carmo Barbosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-2351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Major Joaquim Antônio de Mello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJTR9X8j_wzJQRlw0YBZ7B-Bk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">André Ribeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJh93UjD_wzJQRB5aiNH5V5Jw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nair de Almeida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-5927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Eynaldo Ramos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ8eZQthXwzJQRRwhlVoImmdY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Maria Pereira da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-3642</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Manoel Cembraneli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJyS6UbhXwzJQR4XqDcBhgGmA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-6263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJHa5ZDRXwzJQRwGWGts7uzJY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diva Moreira S. Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-7389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Manoel Antonio Homem de Melo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJIXIauRXwzJQRue-mJQpKuZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Aparecida Rodrigues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-4007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJu3E7Pz7wzJQRwgsJgOzu_Sg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduardo Giovanni de Matos Gomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99608-8058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJW2ApiBXwzJQR2eMqSEfbcbI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniela de Assis Victório da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98825-8832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ9TLqgxXwzJQRz6NjSMJx7_I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Estevão da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3522-4088</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJP0Pq_RTwzJQR_nOVIhdOgNg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vânia Cristina de Jesus Fábio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98127-1558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJCxdwNj7wzJQRGbzZszOtyAk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatiana Ribeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99127-6655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJvaikLT7wzJQRWAkbbNZvPOk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atílio Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98181-3413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJc9bYExXwzJQRT6LCzt2JNW4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarosiahy Laudo Cardoso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3643-1612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ11t5FBXwzJQR18nPTY42_xo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elza N S Bondioli de Oliveira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97406-6067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEGAR NO Nº 425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJi-j6EBXwzJQRN_NR1iQ6-1o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milton Pires Junior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-5364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ek9SLiDDgWx2YXJvIExlbWUsIDIwMiAtIENow6FjYXJhIEdhbGVnYSwgUGluZGFtb25oYW5nYWJhIC0gU1AsIDEyNDIyLTE1MCwgQnJhemlsIhsSGQoUChIJyW8RYBXwzJQRygK0uWkzKggQygE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silvia Eloiza Pires Camargo Leite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98155-0334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regina Célia Carvalho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3648-1230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">José Luiz Romão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3643-1240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FORA DE ORDEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJP4EWCEDwzJQRaIAf43K0S9E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lourdes dos Santos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3642-6262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJ1STNHhXwzJQRVuUCM2fTCiM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valdirene Alves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99660-9881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ChIJi7zfPBXwzJQRPpjsmPc6v7A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -549,6 +1310,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -599,7 +1365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -624,7 +1390,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,18 +1485,18 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="56.04"/>
@@ -776,7 +1554,7 @@
       <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="0" t="n">
         <v>69</v>
       </c>
       <c r="H2" s="2"/>
@@ -939,7 +1717,7 @@
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="0" t="n">
         <v>81</v>
       </c>
       <c r="H8" s="2"/>
@@ -967,7 +1745,7 @@
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="0" t="n">
         <v>168</v>
       </c>
       <c r="H9" s="2"/>
@@ -995,7 +1773,7 @@
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="0" t="n">
         <v>18</v>
       </c>
       <c r="H10" s="2"/>
@@ -1023,7 +1801,7 @@
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="0" t="n">
         <v>22</v>
       </c>
       <c r="H11" s="2"/>
@@ -1051,7 +1829,7 @@
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="0" t="n">
         <v>114</v>
       </c>
       <c r="H12" s="2"/>
@@ -1076,7 +1854,7 @@
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="0" t="n">
         <v>17</v>
       </c>
       <c r="H13" s="2"/>
@@ -1104,7 +1882,7 @@
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="0" t="n">
         <v>44</v>
       </c>
       <c r="H14" s="2"/>
@@ -1129,7 +1907,7 @@
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="0" t="n">
         <v>105</v>
       </c>
       <c r="H15" s="2"/>
@@ -1157,7 +1935,7 @@
       <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="0" t="n">
         <v>84</v>
       </c>
       <c r="H16" s="2"/>
@@ -1185,7 +1963,7 @@
       <c r="F17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="0" t="n">
         <v>113</v>
       </c>
       <c r="H17" s="2"/>
@@ -1548,7 +2326,7 @@
       <c r="G31" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1981,7 +2759,7 @@
       <c r="G48" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I48" s="6" t="s">
+      <c r="I48" s="7" t="s">
         <v>155</v>
       </c>
       <c r="J48" s="4" t="s">
@@ -2023,4 +2801,1951 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J71"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="56.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="185.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>376</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>550</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>442</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>448</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>459</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>523</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>178</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="8" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>449</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>305</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>411</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>422</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>434</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>565</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>460</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>390</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>291</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>469</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>488</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>315</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>284</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>392</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>407</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>280</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="I48" s="7"/>
+      <c r="J48" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>325</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>397</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>417</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>316</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>585</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>155</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>425</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>438</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>439</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>305</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>290</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrigindo nome da rua Rodrigo Romeiro
</commit_message>
<xml_diff>
--- a/src/main/resources/carga-inicial-doadores.xlsx
+++ b/src/main/resources/carga-inicial-doadores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="32"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Crispim - 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -389,6 +389,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  (</t>
     </r>
@@ -399,6 +400,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">LADO)</t>
     </r>
@@ -659,7 +661,7 @@
     <t xml:space="preserve">9782-4443</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Dr. Ruadrigo Ruameiro</t>
+    <t xml:space="preserve">Rua Dr. Rodrigo Romeiro</t>
   </si>
   <si>
     <t xml:space="preserve">ChIJzyZ5WS_wzJQRkZoDZLObjEc</t>
@@ -754,6 +756,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -764,6 +767,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Apt°11 </t>
     </r>
@@ -773,6 +777,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -783,6 +788,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">BLOCO B</t>
     </r>
@@ -866,7 +872,7 @@
     <t xml:space="preserve">3522-8773</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Ruadrigo Ruameiro</t>
+    <t xml:space="preserve">Rua Rodrigo Romeiro</t>
   </si>
   <si>
     <t xml:space="preserve">ChIJIzSRnybwzJQRDykX8_8nVhk</t>
@@ -1133,7 +1139,7 @@
     <t xml:space="preserve">98193-9354</t>
   </si>
   <si>
-    <t xml:space="preserve">Rua Dr.Ruadrigo Ruameiro</t>
+    <t xml:space="preserve">Rua Dr.Rodrigo Romeiro</t>
   </si>
   <si>
     <t xml:space="preserve">Ek5SLiBEci4gUm9kcmlnbyBSb21laXJvLCAxMzYgLSBDcmlzcGltLCBQaW5kYW1vbmhhbmdhYmEgLSBTUCwgMTI0MDItMDYwLCBCcmF6aWwiGxIZChQKEgnDrdupJvDMlBG4f2In4R62mBCIAQ</t>
@@ -2398,6 +2404,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">496  9773-2817 - </t>
     </r>
@@ -2407,6 +2414,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">FILHA NANCY - BUSCAR NO Nº 516</t>
     </r>
@@ -2468,6 +2476,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2478,6 +2487,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> BUSCAR DURANTE A SEMANA</t>
     </r>
@@ -2689,6 +2699,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -2698,6 +2709,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 99118-3779</t>
     </r>
@@ -4679,6 +4691,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -4689,6 +4702,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">AO LADO DO 315</t>
     </r>
@@ -5860,6 +5874,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  </t>
     </r>
@@ -5870,6 +5885,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(VIDRACEIRO</t>
     </r>
@@ -5879,6 +5895,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -6471,6 +6488,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -6480,6 +6498,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -6490,6 +6509,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">AO LADO DO SOS</t>
     </r>
@@ -7003,6 +7023,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Aptº  54</t>
     </r>
@@ -7012,6 +7033,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">     </t>
     </r>
@@ -7022,6 +7044,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> EDIFÍCIO SAMOA</t>
     </r>
@@ -7053,6 +7076,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -7063,6 +7087,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">PEGAR QUINTA OU SEXTA</t>
     </r>
@@ -8258,6 +8283,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -8267,6 +8293,7 @@
         <sz val="14"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1º QUARTEIRÃO</t>
     </r>
@@ -8676,6 +8703,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -8686,6 +8714,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> FUNDOS</t>
     </r>
@@ -8864,6 +8893,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">   </t>
     </r>
@@ -8874,6 +8904,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">FUNDOS</t>
     </r>
@@ -8893,6 +8924,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -8903,6 +8935,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> AO LADO DO Nº 151</t>
     </r>
@@ -9684,7 +9717,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -9721,16 +9754,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -9743,18 +9772,14 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -9762,12 +9787,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -9824,7 +9851,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -9841,35 +9868,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9877,7 +9896,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9964,17 +9983,17 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
@@ -11341,7 +11360,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11394,7 +11413,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11427,7 +11446,7 @@
       <selection pane="topLeft" activeCell="J75" activeCellId="0" sqref="J75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -11749,7 +11768,7 @@
       <c r="G12" s="0" t="n">
         <v>348</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="4" t="s">
         <v>1068</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -12962,7 +12981,7 @@
       <c r="G59" s="0" t="n">
         <v>177</v>
       </c>
-      <c r="I59" s="7"/>
+      <c r="I59" s="4"/>
       <c r="J59" s="2" t="s">
         <v>1211</v>
       </c>
@@ -12989,7 +13008,7 @@
       <c r="G60" s="0" t="n">
         <v>199</v>
       </c>
-      <c r="I60" s="7"/>
+      <c r="I60" s="4"/>
       <c r="J60" s="2" t="s">
         <v>1214</v>
       </c>
@@ -13016,7 +13035,7 @@
       <c r="G61" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="I61" s="7" t="s">
+      <c r="I61" s="4" t="s">
         <v>953</v>
       </c>
       <c r="J61" s="2" t="s">
@@ -13045,7 +13064,7 @@
       <c r="G62" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="I62" s="7"/>
+      <c r="I62" s="4"/>
       <c r="J62" s="2" t="s">
         <v>1220</v>
       </c>
@@ -13101,7 +13120,7 @@
       <c r="G64" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="I64" s="7"/>
+      <c r="I64" s="4"/>
       <c r="J64" s="2" t="s">
         <v>1227</v>
       </c>
@@ -13128,7 +13147,7 @@
       <c r="G65" s="0" t="n">
         <v>107</v>
       </c>
-      <c r="I65" s="7"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="2" t="s">
         <v>1231</v>
       </c>
@@ -13155,7 +13174,7 @@
       <c r="G66" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I66" s="7"/>
+      <c r="I66" s="4"/>
       <c r="J66" s="2" t="s">
         <v>1234</v>
       </c>
@@ -13182,7 +13201,7 @@
       <c r="G67" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="I67" s="7"/>
+      <c r="I67" s="4"/>
       <c r="J67" s="2" t="s">
         <v>1238</v>
       </c>
@@ -13238,7 +13257,7 @@
       <c r="G69" s="0" t="n">
         <v>560</v>
       </c>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2" t="s">
         <v>1245</v>
       </c>
@@ -13450,7 +13469,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -14052,14 +14071,14 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.25"/>
@@ -14455,7 +14474,7 @@
       <c r="H15" s="0" t="s">
         <v>1315</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="3" t="s">
         <v>1316</v>
       </c>
       <c r="J15" s="2" t="s">
@@ -15002,7 +15021,7 @@
       <c r="G36" s="0" t="n">
         <v>163</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="3" t="s">
         <v>1386</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -15063,7 +15082,7 @@
       <c r="H38" s="0" t="s">
         <v>1394</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="3" t="s">
         <v>953</v>
       </c>
       <c r="J38" s="2" t="s">
@@ -15282,7 +15301,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15335,7 +15354,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15368,7 +15387,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -15973,7 +15992,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16026,7 +16045,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16059,7 +16078,7 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -17000,7 +17019,7 @@
       <c r="G35" s="0" t="n">
         <v>130</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="7" t="s">
         <v>1591</v>
       </c>
       <c r="J35" s="2" t="s">
@@ -17091,7 +17110,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17144,7 +17163,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17177,7 +17196,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -17456,7 +17475,7 @@
       <c r="G10" s="0" t="n">
         <v>143</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="8" t="s">
         <v>1627</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -18223,7 +18242,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18276,7 +18295,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18309,7 +18328,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -18478,7 +18497,7 @@
       <c r="G6" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="8" t="s">
         <v>1731</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -18847,7 +18866,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18900,7 +18919,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18933,7 +18952,7 @@
       <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -20151,7 +20170,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20204,7 +20223,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20237,11 +20256,11 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.97"/>
@@ -20583,7 +20602,7 @@
       <c r="G13" s="0" t="n">
         <v>357</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="2" t="s">
         <v>1947</v>
       </c>
@@ -20910,7 +20929,7 @@
       <c r="G26" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="4"/>
       <c r="J26" s="2" t="s">
         <v>1988</v>
       </c>
@@ -21312,7 +21331,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -21545,7 +21564,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21598,7 +21617,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21627,11 +21646,11 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -22008,7 +22027,7 @@
       <c r="G14" s="0" t="n">
         <v>162</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>222</v>
       </c>
       <c r="J14" s="2" t="s">
@@ -23087,7 +23106,7 @@
       <c r="G56" s="0" t="n">
         <v>588</v>
       </c>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2" t="s">
         <v>353</v>
       </c>
@@ -23273,7 +23292,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23306,7 +23325,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -23579,7 +23598,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23632,7 +23651,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23665,7 +23684,7 @@
       <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -23924,7 +23943,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23977,7 +23996,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24010,7 +24029,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -24335,7 +24354,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24388,7 +24407,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24421,7 +24440,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -24657,7 +24676,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24710,7 +24729,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24743,7 +24762,7 @@
       <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -26362,7 +26381,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26395,7 +26414,7 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -26808,7 +26827,7 @@
       <c r="D15" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>2318</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -26836,7 +26855,7 @@
       <c r="D16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>2318</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -27060,7 +27079,7 @@
       <c r="G24" s="0" t="n">
         <v>434</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="4" t="s">
         <v>953</v>
       </c>
       <c r="J24" s="2" t="s">
@@ -27141,7 +27160,7 @@
       <c r="G27" s="0" t="n">
         <v>460</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="4" t="s">
         <v>2357</v>
       </c>
       <c r="J27" s="2" t="s">
@@ -27317,7 +27336,7 @@
       <c r="D34" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="4" t="s">
         <v>2379</v>
       </c>
       <c r="F34" s="6" t="s">
@@ -27378,7 +27397,7 @@
       <c r="G36" s="0" t="n">
         <v>113</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="4" t="s">
         <v>2389</v>
       </c>
       <c r="J36" s="2" t="s">
@@ -27702,7 +27721,7 @@
       <c r="G48" s="0" t="n">
         <v>288</v>
       </c>
-      <c r="I48" s="7"/>
+      <c r="I48" s="4"/>
       <c r="J48" s="2" t="s">
         <v>2429</v>
       </c>
@@ -27830,7 +27849,7 @@
       <c r="G53" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="I53" s="7" t="s">
+      <c r="I53" s="4" t="s">
         <v>2389</v>
       </c>
       <c r="J53" s="2" t="s">
@@ -27917,7 +27936,7 @@
       <c r="G56" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="I56" s="4" t="s">
         <v>2389</v>
       </c>
       <c r="J56" s="2" t="s">
@@ -28261,7 +28280,7 @@
       <c r="G69" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="I69" s="7" t="s">
+      <c r="I69" s="4" t="s">
         <v>2494</v>
       </c>
       <c r="J69" s="2" t="s">
@@ -28342,7 +28361,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -28414,7 +28433,7 @@
       <c r="I2" s="6" t="s">
         <v>2507</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>2508</v>
       </c>
     </row>
@@ -28440,7 +28459,7 @@
       <c r="G3" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="10" t="s">
         <v>2512</v>
       </c>
     </row>
@@ -28466,7 +28485,7 @@
       <c r="G4" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="10" t="s">
         <v>2515</v>
       </c>
     </row>
@@ -28492,7 +28511,7 @@
       <c r="G5" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>2519</v>
       </c>
     </row>
@@ -28518,7 +28537,7 @@
       <c r="G6" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="11" t="s">
         <v>2523</v>
       </c>
     </row>
@@ -28547,7 +28566,7 @@
       <c r="I7" s="0" t="s">
         <v>953</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="10" t="s">
         <v>2527</v>
       </c>
     </row>
@@ -28575,7 +28594,7 @@
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="9" t="s">
         <v>2529</v>
       </c>
     </row>
@@ -28603,7 +28622,7 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="9" t="s">
         <v>2532</v>
       </c>
     </row>
@@ -28631,7 +28650,7 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="9" t="s">
         <v>2535</v>
       </c>
     </row>
@@ -28659,7 +28678,7 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="9" t="s">
         <v>2538</v>
       </c>
     </row>
@@ -28687,7 +28706,7 @@
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="9" t="s">
         <v>2541</v>
       </c>
     </row>
@@ -28712,7 +28731,7 @@
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="9" t="s">
         <v>2544</v>
       </c>
     </row>
@@ -28740,7 +28759,7 @@
       </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="9" t="s">
         <v>2547</v>
       </c>
     </row>
@@ -28765,7 +28784,7 @@
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="10" t="s">
         <v>2549</v>
       </c>
     </row>
@@ -28793,7 +28812,7 @@
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="9" t="s">
         <v>2552</v>
       </c>
     </row>
@@ -28821,7 +28840,7 @@
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="9" t="s">
         <v>2556</v>
       </c>
     </row>
@@ -28844,7 +28863,7 @@
       <c r="G18" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="9" t="s">
         <v>2559</v>
       </c>
     </row>
@@ -28870,7 +28889,7 @@
       <c r="G19" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="9" t="s">
         <v>2562</v>
       </c>
     </row>
@@ -28896,7 +28915,7 @@
       <c r="G20" s="0" t="n">
         <v>139</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="9" t="s">
         <v>2565</v>
       </c>
     </row>
@@ -28922,7 +28941,7 @@
       <c r="G21" s="0" t="n">
         <v>265</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="9" t="s">
         <v>2568</v>
       </c>
     </row>
@@ -28948,7 +28967,7 @@
       <c r="G22" s="0" t="n">
         <v>329</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="9" t="s">
         <v>2571</v>
       </c>
     </row>
@@ -28974,7 +28993,7 @@
       <c r="I23" s="0" t="s">
         <v>953</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="10" t="s">
         <v>2574</v>
       </c>
     </row>
@@ -28997,7 +29016,7 @@
       <c r="G24" s="0" t="n">
         <v>511</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="10" t="s">
         <v>2576</v>
       </c>
     </row>
@@ -29023,7 +29042,7 @@
       <c r="G25" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" s="10" t="s">
         <v>2579</v>
       </c>
     </row>
@@ -29046,7 +29065,7 @@
       <c r="G26" s="0" t="n">
         <v>235</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="J26" s="10" t="s">
         <v>2581</v>
       </c>
     </row>
@@ -29075,7 +29094,7 @@
       <c r="I27" s="0" t="s">
         <v>2584</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="J27" s="10" t="s">
         <v>2585</v>
       </c>
     </row>
@@ -29101,7 +29120,7 @@
       <c r="G28" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="10" t="s">
         <v>2588</v>
       </c>
     </row>
@@ -29127,7 +29146,7 @@
       <c r="G29" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="J29" s="10" t="s">
         <v>2591</v>
       </c>
     </row>
@@ -29153,7 +29172,7 @@
       <c r="G30" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J30" s="10" t="s">
         <v>2594</v>
       </c>
     </row>
@@ -29179,7 +29198,7 @@
       <c r="G31" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="12" t="s">
         <v>2597</v>
       </c>
     </row>
@@ -29205,7 +29224,7 @@
       <c r="G32" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="J32" s="12" t="s">
+      <c r="J32" s="10" t="s">
         <v>2600</v>
       </c>
     </row>
@@ -29231,7 +29250,7 @@
       <c r="G33" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="J33" s="11" t="s">
+      <c r="J33" s="9" t="s">
         <v>2603</v>
       </c>
     </row>
@@ -29254,7 +29273,7 @@
       <c r="G34" s="0" t="n">
         <v>98</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="10" t="s">
         <v>2605</v>
       </c>
     </row>
@@ -29280,7 +29299,7 @@
       <c r="G35" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="10" t="s">
         <v>2609</v>
       </c>
     </row>
@@ -29306,7 +29325,7 @@
       <c r="G36" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="J36" s="11" t="s">
+      <c r="J36" s="9" t="s">
         <v>2612</v>
       </c>
     </row>
@@ -29332,7 +29351,7 @@
       <c r="G37" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="10" t="s">
         <v>2615</v>
       </c>
     </row>
@@ -29358,7 +29377,7 @@
       <c r="G38" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="J38" s="9" t="s">
         <v>2618</v>
       </c>
     </row>
@@ -29384,7 +29403,7 @@
       <c r="G39" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="J39" s="11" t="s">
+      <c r="J39" s="9" t="s">
         <v>2621</v>
       </c>
     </row>
@@ -29410,7 +29429,7 @@
       <c r="G40" s="0" t="n">
         <v>205</v>
       </c>
-      <c r="J40" s="11" t="s">
+      <c r="J40" s="9" t="s">
         <v>2624</v>
       </c>
     </row>
@@ -29433,7 +29452,7 @@
       <c r="G41" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="J41" s="10" t="s">
         <v>2626</v>
       </c>
     </row>
@@ -29456,7 +29475,7 @@
       <c r="G42" s="0" t="n">
         <v>117</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" s="10" t="s">
         <v>2628</v>
       </c>
     </row>
@@ -29482,7 +29501,7 @@
       <c r="G43" s="0" t="n">
         <v>275</v>
       </c>
-      <c r="J43" s="12" t="s">
+      <c r="J43" s="10" t="s">
         <v>2631</v>
       </c>
     </row>
@@ -29508,7 +29527,7 @@
       <c r="G44" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="J44" s="10" t="s">
         <v>2634</v>
       </c>
     </row>
@@ -29534,7 +29553,7 @@
       <c r="G45" s="0" t="n">
         <v>148</v>
       </c>
-      <c r="J45" s="12" t="s">
+      <c r="J45" s="10" t="s">
         <v>2637</v>
       </c>
     </row>
@@ -29560,7 +29579,7 @@
       <c r="G46" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J46" s="12" t="s">
+      <c r="J46" s="10" t="s">
         <v>2640</v>
       </c>
     </row>
@@ -29586,7 +29605,7 @@
       <c r="G47" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="10" t="s">
         <v>2643</v>
       </c>
     </row>
@@ -29612,10 +29631,10 @@
       <c r="G48" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I48" s="4" t="s">
         <v>2646</v>
       </c>
-      <c r="J48" s="12" t="s">
+      <c r="J48" s="10" t="s">
         <v>2647</v>
       </c>
     </row>
@@ -29641,7 +29660,7 @@
       <c r="G49" s="0" t="n">
         <v>150</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="10" t="s">
         <v>2650</v>
       </c>
     </row>
@@ -29667,11 +29686,11 @@
       <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.97"/>
@@ -29842,7 +29861,7 @@
       <c r="G6" s="0" t="n">
         <v>955</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>2669</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -31115,7 +31134,7 @@
       <c r="G55" s="0" t="n">
         <v>129</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="4"/>
       <c r="J55" s="2" t="s">
         <v>2819</v>
       </c>
@@ -31443,7 +31462,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="6"/>
-      <c r="I68" s="7"/>
+      <c r="I68" s="4"/>
       <c r="J68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31476,11 +31495,11 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.97"/>
@@ -32649,7 +32668,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32702,7 +32721,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32735,7 +32754,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -33311,7 +33330,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33364,7 +33383,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33397,7 +33416,7 @@
       <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -34852,7 +34871,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34905,7 +34924,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34938,7 +34957,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -35280,7 +35299,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35333,7 +35352,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35366,7 +35385,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -35602,7 +35621,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35655,7 +35674,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35688,7 +35707,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -36050,7 +36069,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F54" s="6"/>
-      <c r="I54" s="7"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36103,7 +36122,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="6"/>
-      <c r="I67" s="7"/>
+      <c r="I67" s="4"/>
       <c r="J67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36132,11 +36151,11 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -36372,7 +36391,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36425,7 +36444,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36458,7 +36477,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -36760,7 +36779,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36813,7 +36832,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36846,7 +36865,7 @@
       <selection pane="topLeft" activeCell="F71" activeCellId="0" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -36914,7 +36933,7 @@
       <c r="G2" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="3" t="s">
         <v>570</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -38143,7 +38162,7 @@
       <c r="I50" s="0" t="s">
         <v>718</v>
       </c>
-      <c r="J50" s="7" t="s">
+      <c r="J50" s="4" t="s">
         <v>719</v>
       </c>
     </row>
@@ -38299,7 +38318,7 @@
       <c r="G56" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2" t="s">
         <v>571</v>
       </c>
@@ -38508,7 +38527,7 @@
       <c r="G64" s="0" t="n">
         <v>445</v>
       </c>
-      <c r="I64" s="9" t="s">
+      <c r="I64" s="3" t="s">
         <v>759</v>
       </c>
       <c r="J64" s="2" t="s">
@@ -38641,7 +38660,7 @@
       <c r="G69" s="0" t="n">
         <v>352</v>
       </c>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2" t="s">
         <v>774</v>
       </c>
@@ -38723,7 +38742,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -38732,7 +38751,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="185.91"/>
   </cols>
@@ -38843,7 +38862,7 @@
       <c r="G4" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="3" t="s">
         <v>794</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -39760,7 +39779,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39813,7 +39832,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39846,7 +39865,7 @@
       <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -40289,7 +40308,7 @@
       <c r="G17" s="0" t="n">
         <v>687</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="3" t="s">
         <v>953</v>
       </c>
       <c r="J17" s="2" t="s">
@@ -40530,7 +40549,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40583,7 +40602,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40616,7 +40635,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -40947,7 +40966,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41000,7 +41019,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41033,7 +41052,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -41170,7 +41189,7 @@
       <c r="D5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="3" t="s">
         <v>1009</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -41179,7 +41198,7 @@
       <c r="G5" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="3" t="s">
         <v>1010</v>
       </c>
       <c r="J5" s="2" t="s">
@@ -41482,7 +41501,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F56" s="6"/>
-      <c r="I56" s="7"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41535,7 +41554,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="6"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>